<commit_message>
21/07/2020 Update API List
</commit_message>
<xml_diff>
--- a/Restful-api.xlsx
+++ b/Restful-api.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e841f78043019b2e/文件/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\PycharmProjects\Restful-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="315" documentId="8_{7151B69C-99C6-4B42-9BDC-F13D465BD89C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D371CC07-9F97-40EB-A2DD-69207E14C383}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA314980-9441-41C2-92C6-663311137121}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{396F9068-CCEB-4AF1-BF68-127B62764BF9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{396F9068-CCEB-4AF1-BF68-127B62764BF9}"/>
   </bookViews>
   <sheets>
-    <sheet name="test.py" sheetId="1" r:id="rId1"/>
-    <sheet name="工作表1" sheetId="2" r:id="rId2"/>
+    <sheet name="Complex Test Case" sheetId="1" r:id="rId1"/>
+    <sheet name="Unit Test Case" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="152">
   <si>
     <t>Function Name</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -316,58 +316,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Key</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Value</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Category</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>home</t>
-  </si>
-  <si>
-    <t>snap_id</t>
-  </si>
-  <si>
-    <t>{snap_id}</t>
-  </si>
-  <si>
-    <t>order</t>
-  </si>
-  <si>
-    <t>{DESC|ASC}</t>
-  </si>
-  <si>
-    <t>orderby</t>
-  </si>
-  <si>
-    <t>{creation|popularity}</t>
-  </si>
-  <si>
-    <t>filter</t>
-  </si>
-  <si>
-    <t>{editorpick}</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>search</t>
-  </si>
-  <si>
-    <t>q</t>
-  </si>
-  <si>
-    <t>{keyword}</t>
-  </si>
-  <si>
-    <t>product</t>
-  </si>
-  <si>
     <t>Get user follower &amp; following count</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -479,6 +427,226 @@
   </si>
   <si>
     <t>Check the like result equal or larger than 0</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>API</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status Code</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Login</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Logout</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Register</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Done?</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Method</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Normal</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Missing email</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Invalid email</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Missing password</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Existing email</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get Snap</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Missing Title</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Missing Description</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Missing Image Name</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Missing Image Body</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Missing Ref id</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Create Snap</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Missing snap_id</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get Single Snap</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unexisting snap_id</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status Code: 200 &amp; Return null</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status Code: 413 &amp; Return html</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>7MB image</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>9MB image</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>11MB image</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Define the query parameter for get_snap, search_snap, get_product API</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get Snap, Search Snap and Get Product</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get the snap_id of the last item from the result list</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pass the snap_id into query</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get snap info after login</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remove Snap</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Logout and Remove normal snap</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Logout and Create normal snap</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get Product of a snap</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Search snap</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Empty query</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Invalid snap_id</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Incorrect order parameter</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get comment of a snap</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Post Comment</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Missing comment</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Logout and post comment normally</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Missing snap_id for home</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Missing snap_id for search</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Missing snap_id for product</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Logout and get snap info after login normally</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remove a snap from a snap</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Not find a suitable snap_product_id for testing the snap remove</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Missing snap_product_id</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Logout and remove a snap from a snap</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unexisting snap_product_id</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -579,8 +747,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -896,10 +1064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{772D621B-BAA2-482D-AA82-4BEFD6A2E911}">
-  <dimension ref="A1:C138"/>
+  <dimension ref="A1:C145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="B138" sqref="B138"/>
+    <sheetView topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1150,130 +1318,125 @@
       <c r="A51" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="B51" t="s">
+        <v>126</v>
+      </c>
       <c r="C51" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="B52" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="B53" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="B54" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="B55" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="B56" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="B57" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
-      <c r="C52" t="s">
+    <row r="63" spans="1:3">
+      <c r="C63" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C55" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="C56" t="s">
+    <row r="67" spans="1:3">
+      <c r="A67" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C67" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="C68" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C60" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="C61" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="2" t="s">
+    <row r="73" spans="1:3">
+      <c r="A73" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B73" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
-      <c r="B67" t="s">
+    <row r="74" spans="1:3">
+      <c r="B74" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
-      <c r="B68" t="s">
+    <row r="75" spans="1:3">
+      <c r="B75" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
-      <c r="A71" s="2" t="s">
+    <row r="78" spans="1:3">
+      <c r="A78" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B78" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
-      <c r="A72" s="2"/>
-      <c r="B72" s="4" t="s">
+    <row r="79" spans="1:3">
+      <c r="A79" s="2"/>
+      <c r="B79" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="2"/>
-      <c r="B73" s="4" t="s">
+    <row r="80" spans="1:3">
+      <c r="A80" s="2"/>
+      <c r="B80" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
-      <c r="B74" t="s">
+    <row r="81" spans="1:2">
+      <c r="B81" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
-      <c r="B75" s="4" t="s">
+    <row r="82" spans="1:2">
+      <c r="B82" s="4" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
-      <c r="B76" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="B77" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
-      <c r="B78" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2">
-      <c r="A80" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B80" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="B81" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="B82" s="6" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="B83" s="4" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="B84" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1281,243 +1444,245 @@
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
-      <c r="B86" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
     <row r="87" spans="1:2">
-      <c r="B87" t="s">
-        <v>62</v>
+      <c r="A87" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="B88" s="4" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="89" spans="1:2">
-      <c r="B89" t="s">
-        <v>11</v>
+      <c r="B89" s="6" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="B90" s="4" t="s">
-        <v>63</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="B91" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="92" spans="1:2">
-      <c r="A92" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B92" s="6" t="s">
-        <v>83</v>
+      <c r="B92" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="B93" s="4" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="B94" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="B95" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="B96" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
-      <c r="B95" t="s">
-        <v>84</v>
-      </c>
-    </row>
     <row r="97" spans="1:2">
-      <c r="A97" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B97" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2">
-      <c r="B98" s="4" t="s">
-        <v>86</v>
+      <c r="B97" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="99" spans="1:2">
-      <c r="B99" s="4" t="s">
-        <v>89</v>
+      <c r="A99" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B99" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="B100" s="4" t="s">
-        <v>88</v>
+        <v>12</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="B101" t="s">
-        <v>87</v>
+        <v>11</v>
       </c>
     </row>
     <row r="102" spans="1:2">
-      <c r="B102" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2">
-      <c r="B103" s="4" t="s">
-        <v>90</v>
+      <c r="B102" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B104" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="105" spans="1:2">
-      <c r="A105" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B105" s="6" t="s">
-        <v>92</v>
+      <c r="B105" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="B106" s="4" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
     </row>
     <row r="107" spans="1:2">
-      <c r="B107" t="s">
-        <v>93</v>
+      <c r="B107" s="4" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="108" spans="1:2">
-      <c r="B108" s="4" t="s">
-        <v>12</v>
+      <c r="B108" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="B109" s="4" t="s">
-        <v>94</v>
+        <v>29</v>
       </c>
     </row>
     <row r="110" spans="1:2">
-      <c r="B110" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2">
-      <c r="B111" s="4" t="s">
-        <v>29</v>
+      <c r="B110" s="4" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="112" spans="1:2">
-      <c r="B112" t="s">
-        <v>93</v>
+      <c r="A112" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B112" s="6" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="B113" s="4" t="s">
-        <v>96</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="B114" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="115" spans="1:2">
-      <c r="A115" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B115" s="6" t="s">
-        <v>98</v>
+      <c r="B115" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="B116" s="4" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="B117" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="B118" s="4" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row r="119" spans="1:2">
-      <c r="B119" s="4" t="s">
-        <v>100</v>
+      <c r="B119" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="120" spans="1:2">
-      <c r="B120" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2">
-      <c r="B121" s="4" t="s">
-        <v>29</v>
+      <c r="B120" s="4" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="122" spans="1:2">
-      <c r="B122" t="s">
-        <v>93</v>
+      <c r="A122" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B122" s="6" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="B123" s="4" t="s">
-        <v>101</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="B124" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="125" spans="1:2">
-      <c r="A125" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B125" s="6" t="s">
-        <v>103</v>
+      <c r="B125" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="B126" s="4" t="s">
-        <v>12</v>
+        <v>84</v>
       </c>
     </row>
     <row r="127" spans="1:2">
-      <c r="B127" s="4" t="s">
-        <v>105</v>
+      <c r="B127" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="B128" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="129" spans="1:2">
-      <c r="A129" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="B129" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="B130" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B132" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="B133" s="4" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2">
-      <c r="B131" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2">
-      <c r="A133" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B133" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="B134" s="4" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" s="2" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="B136" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -1527,7 +1692,38 @@
     </row>
     <row r="138" spans="1:2">
       <c r="B138" s="4" t="s">
-        <v>112</v>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B140" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="B141" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B143" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="B144" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="145" spans="2:2">
+      <c r="B145" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1538,109 +1734,675 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0FB8395-3546-4B63-9E36-2AC157E5E294}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="14.875" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="23.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="40.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="55.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" t="s">
-        <v>67</v>
+        <v>97</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>98</v>
       </c>
       <c r="C1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="B3" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="B4" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="B5" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="B7" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="B8" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="B9" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>72</v>
+        <v>104</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="6">
+        <v>200</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="B3" s="6">
+        <v>400</v>
+      </c>
+      <c r="C3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="B4" s="6">
+        <v>400</v>
+      </c>
+      <c r="C4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="B5" s="6">
+        <v>404</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="6">
+        <v>200</v>
+      </c>
+      <c r="C7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="B8" s="6">
+        <v>401</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="6">
+        <v>200</v>
+      </c>
+      <c r="C10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="B11" s="6">
+        <v>400</v>
+      </c>
+      <c r="C11" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="B12" s="6">
+        <v>400</v>
+      </c>
+      <c r="C12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="B13" s="6">
+        <v>400</v>
+      </c>
+      <c r="C13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="B14" s="6">
+        <v>400</v>
+      </c>
+      <c r="C14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16" s="6">
+        <v>200</v>
+      </c>
+      <c r="C16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="B17" s="6">
+        <v>400</v>
+      </c>
+      <c r="C17" t="s">
+        <v>118</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="B18" s="6">
+        <v>404</v>
+      </c>
+      <c r="C18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>119</v>
+      </c>
+      <c r="B20" s="6">
+        <v>200</v>
+      </c>
+      <c r="C20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="B21" s="6">
+        <v>400</v>
+      </c>
+      <c r="C21" t="s">
+        <v>118</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="B22" s="6">
+        <v>400</v>
+      </c>
+      <c r="C22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25" s="6">
+        <v>200</v>
+      </c>
+      <c r="C25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="B26" s="6">
+        <v>400</v>
+      </c>
+      <c r="C26" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="B27" s="6">
+        <v>400</v>
+      </c>
+      <c r="C27" t="s">
+        <v>113</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="B28" s="6">
+        <v>400</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="B29" s="6">
+        <v>400</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="B30" s="6">
+        <v>400</v>
+      </c>
+      <c r="C30" t="s">
+        <v>116</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="B31" s="6">
+        <v>401</v>
+      </c>
+      <c r="C31" t="s">
+        <v>125</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E31" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="B32" s="6">
+        <v>401</v>
+      </c>
+      <c r="C32" t="s">
+        <v>124</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E32" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="B33" s="6">
+        <v>401</v>
+      </c>
+      <c r="C33" t="s">
+        <v>123</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="B34" s="6">
+        <v>401</v>
+      </c>
+      <c r="C34" t="s">
+        <v>133</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>131</v>
+      </c>
+      <c r="B36" s="6">
+        <v>204</v>
+      </c>
+      <c r="C36" t="s">
+        <v>105</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="B37" s="6">
+        <v>404</v>
+      </c>
+      <c r="C37" t="s">
+        <v>118</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="B38" s="6">
+        <v>404</v>
+      </c>
+      <c r="C38" t="s">
+        <v>120</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="B39" s="6">
+        <v>401</v>
+      </c>
+      <c r="C39" t="s">
+        <v>132</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41" s="6">
+        <v>200</v>
+      </c>
+      <c r="C41" t="s">
+        <v>105</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="B42" s="6">
+        <v>404</v>
+      </c>
+      <c r="C42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="B43" s="6">
+        <v>404</v>
+      </c>
+      <c r="C43" t="s">
+        <v>120</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>135</v>
+      </c>
+      <c r="B45" s="6">
+        <v>200</v>
+      </c>
+      <c r="C45" t="s">
+        <v>105</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="B46" s="6">
+        <v>200</v>
+      </c>
+      <c r="C46" t="s">
+        <v>136</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="B47" s="6">
+        <v>500</v>
+      </c>
+      <c r="C47" t="s">
+        <v>138</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>139</v>
+      </c>
+      <c r="B49" s="6">
+        <v>200</v>
+      </c>
+      <c r="C49" t="s">
+        <v>105</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="B50" s="6">
+        <v>404</v>
+      </c>
+      <c r="C50" t="s">
+        <v>118</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="B51" s="6">
+        <v>404</v>
+      </c>
+      <c r="C51" t="s">
+        <v>137</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>140</v>
+      </c>
+      <c r="B53" s="6">
+        <v>201</v>
+      </c>
+      <c r="C53" t="s">
+        <v>105</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="B54" s="6">
+        <v>400</v>
+      </c>
+      <c r="C54" t="s">
+        <v>141</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="B55" s="6">
+        <v>404</v>
+      </c>
+      <c r="C55" t="s">
+        <v>118</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="B56" s="6">
+        <v>404</v>
+      </c>
+      <c r="C56" t="s">
+        <v>120</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="B57" s="6">
+        <v>401</v>
+      </c>
+      <c r="C57" t="s">
+        <v>142</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" t="s">
+        <v>130</v>
+      </c>
+      <c r="B59" s="6">
+        <v>200</v>
+      </c>
+      <c r="C59" t="s">
+        <v>105</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="B60" s="6">
+        <v>400</v>
+      </c>
+      <c r="C60" t="s">
+        <v>143</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="B61" s="6">
+        <v>400</v>
+      </c>
+      <c r="C61" t="s">
+        <v>144</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="B62" s="6">
+        <v>400</v>
+      </c>
+      <c r="C62" t="s">
+        <v>145</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="B63" s="6">
+        <v>401</v>
+      </c>
+      <c r="C63" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>147</v>
+      </c>
+      <c r="B65" s="6">
+        <v>204</v>
+      </c>
+      <c r="C65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E65" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="B66" s="6">
+        <v>404</v>
+      </c>
+      <c r="C66" t="s">
+        <v>149</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="B67" s="6">
+        <v>404</v>
+      </c>
+      <c r="C67" t="s">
+        <v>151</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="B68" s="6">
+        <v>401</v>
+      </c>
+      <c r="C68" t="s">
+        <v>150</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
23/07/2020 Update Unit-test Api
</commit_message>
<xml_diff>
--- a/Restful-api.xlsx
+++ b/Restful-api.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\PycharmProjects\Restful-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA314980-9441-41C2-92C6-663311137121}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2AB059-E2E9-4B70-BE42-486846AAFAF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{396F9068-CCEB-4AF1-BF68-127B62764BF9}"/>
+    <workbookView xWindow="0" yWindow="4215" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{396F9068-CCEB-4AF1-BF68-127B62764BF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Complex Test Case" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="175">
   <si>
     <t>Function Name</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -647,6 +647,98 @@
   </si>
   <si>
     <t>Unexisting snap_product_id</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get snaps by snap product id</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unexisting user_id</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Missing user_id</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Change password</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Missing current password</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Missing new password</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Logout and Change password</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Invalid new password</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Invalid current password</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Update user profile</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Missing username</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Invalid username</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>over 300 character bio</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Logout and update</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Invalid user_id</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unauthorized user_id</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>10kB image</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Firstname = 'Testing'</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Self user_id</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Another valid user_id</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Missing image body</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Invalid image body</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Missing image name</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -1734,10 +1826,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0FB8395-3546-4B63-9E36-2AC157E5E294}">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2059,7 +2151,7 @@
         <v>124</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E32" t="s">
         <v>122</v>
@@ -2402,6 +2494,307 @@
         <v>150</v>
       </c>
       <c r="D68" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>152</v>
+      </c>
+      <c r="B70" s="6">
+        <v>200</v>
+      </c>
+      <c r="C70" t="s">
+        <v>105</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="B71" s="6">
+        <v>404</v>
+      </c>
+      <c r="C71" t="s">
+        <v>151</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="B72" s="6">
+        <v>404</v>
+      </c>
+      <c r="C72" t="s">
+        <v>149</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B74" s="6">
+        <v>200</v>
+      </c>
+      <c r="C74" t="s">
+        <v>170</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="B75" s="6">
+        <v>200</v>
+      </c>
+      <c r="C75" t="s">
+        <v>171</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="B76" s="6">
+        <v>404</v>
+      </c>
+      <c r="C76" t="s">
+        <v>153</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="B77" s="6">
+        <v>404</v>
+      </c>
+      <c r="C77" t="s">
+        <v>154</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>155</v>
+      </c>
+      <c r="B79" s="6">
+        <v>200</v>
+      </c>
+      <c r="C79" t="s">
+        <v>105</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="B80" s="6">
+        <v>400</v>
+      </c>
+      <c r="C80" t="s">
+        <v>156</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="B81" s="6">
+        <v>400</v>
+      </c>
+      <c r="C81" t="s">
+        <v>157</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="B82" s="6">
+        <v>400</v>
+      </c>
+      <c r="C82" t="s">
+        <v>159</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="B83" s="6">
+        <v>401</v>
+      </c>
+      <c r="C83" t="s">
+        <v>167</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="B84" s="6">
+        <v>401</v>
+      </c>
+      <c r="C84" t="s">
+        <v>158</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="B85" s="6">
+        <v>404</v>
+      </c>
+      <c r="C85" t="s">
+        <v>160</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" t="s">
+        <v>161</v>
+      </c>
+      <c r="B87" s="6">
+        <v>200</v>
+      </c>
+      <c r="C87" t="s">
+        <v>169</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="B88" s="6">
+        <v>200</v>
+      </c>
+      <c r="C88" t="s">
+        <v>162</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="B89" s="6">
+        <v>200</v>
+      </c>
+      <c r="C89" t="s">
+        <v>163</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="B90" s="6">
+        <v>200</v>
+      </c>
+      <c r="C90" t="s">
+        <v>164</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="B91" s="6">
+        <v>200</v>
+      </c>
+      <c r="C91" t="s">
+        <v>165</v>
+      </c>
+      <c r="D91" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="B92" s="6">
+        <v>200</v>
+      </c>
+      <c r="C92" t="s">
+        <v>167</v>
+      </c>
+      <c r="D92" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="B93" s="6">
+        <v>200</v>
+      </c>
+      <c r="C93" t="s">
+        <v>154</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="B94" s="6">
+        <v>200</v>
+      </c>
+      <c r="C94" t="s">
+        <v>166</v>
+      </c>
+      <c r="D94" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" t="s">
+        <v>60</v>
+      </c>
+      <c r="B96" s="6">
+        <v>200</v>
+      </c>
+      <c r="C96" t="s">
+        <v>168</v>
+      </c>
+      <c r="D96" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4">
+      <c r="B97" s="6">
+        <v>400</v>
+      </c>
+      <c r="C97" t="s">
+        <v>174</v>
+      </c>
+      <c r="D97" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4">
+      <c r="B98" s="6">
+        <v>400</v>
+      </c>
+      <c r="C98" t="s">
+        <v>172</v>
+      </c>
+      <c r="D98" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4">
+      <c r="B99" s="6">
+        <v>400</v>
+      </c>
+      <c r="C99" t="s">
+        <v>173</v>
+      </c>
+      <c r="D99" s="6" t="s">
         <v>103</v>
       </c>
     </row>

</xml_diff>

<commit_message>
24/07/2020 Update Unit-test Api
</commit_message>
<xml_diff>
--- a/Restful-api.xlsx
+++ b/Restful-api.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\PycharmProjects\Restful-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2AB059-E2E9-4B70-BE42-486846AAFAF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5FF97A-ACB4-42D9-9E5E-25B8A7647A6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="4215" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{396F9068-CCEB-4AF1-BF68-127B62764BF9}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Unit Test Case" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -746,7 +747,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1162,14 +1163,14 @@
       <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.375" customWidth="1"/>
     <col min="2" max="2" width="70" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1180,7 +1181,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1188,27 +1189,27 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -1216,17 +1217,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
@@ -1234,32 +1235,32 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
@@ -1267,17 +1268,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -1285,37 +1286,37 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>36</v>
       </c>
@@ -1326,7 +1327,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>32</v>
       </c>
@@ -1334,12 +1335,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>19</v>
       </c>
@@ -1347,17 +1348,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -1365,17 +1366,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>38</v>
       </c>
@@ -1383,12 +1384,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>42</v>
       </c>
@@ -1396,17 +1397,17 @@
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>46</v>
       </c>
@@ -1417,37 +1418,37 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B57" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>65</v>
       </c>
@@ -1455,12 +1456,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>66</v>
       </c>
@@ -1468,12 +1469,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>10</v>
       </c>
@@ -1481,17 +1482,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>51</v>
       </c>
@@ -1499,44 +1500,44 @@
         <v>52</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B82" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B83" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B85" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>58</v>
       </c>
@@ -1544,57 +1545,57 @@
         <v>59</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B88" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B89" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B90" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B92" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B93" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B95" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B97" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>64</v>
       </c>
@@ -1602,22 +1603,22 @@
         <v>67</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B100" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>13</v>
       </c>
@@ -1625,37 +1626,37 @@
         <v>69</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B105" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B106" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B107" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B109" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B110" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>75</v>
       </c>
@@ -1663,47 +1664,47 @@
         <v>76</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B113" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B115" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B116" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B118" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B120" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>81</v>
       </c>
@@ -1711,47 +1712,47 @@
         <v>82</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B123" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="125" spans="1:2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B125" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="126" spans="1:2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B126" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B128" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="129" spans="1:2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="130" spans="1:2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B130" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="132" spans="1:2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>86</v>
       </c>
@@ -1759,17 +1760,17 @@
         <v>87</v>
       </c>
     </row>
-    <row r="133" spans="1:2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B133" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="134" spans="1:2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B134" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="136" spans="1:2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>88</v>
       </c>
@@ -1777,17 +1778,17 @@
         <v>90</v>
       </c>
     </row>
-    <row r="137" spans="1:2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B137" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="138" spans="1:2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B138" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="140" spans="1:2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>92</v>
       </c>
@@ -1795,12 +1796,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="141" spans="1:2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B141" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="143" spans="1:2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>94</v>
       </c>
@@ -1808,12 +1809,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="144" spans="1:2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B144" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="145" spans="2:2">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B145" s="4" t="s">
         <v>96</v>
       </c>
@@ -1832,7 +1833,7 @@
       <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.125" style="6" customWidth="1"/>
@@ -1841,7 +1842,7 @@
     <col min="5" max="5" width="55.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>97</v>
       </c>
@@ -1858,7 +1859,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -1872,7 +1873,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="6">
         <v>400</v>
       </c>
@@ -1883,7 +1884,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="6">
         <v>400</v>
       </c>
@@ -1894,7 +1895,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="6">
         <v>404</v>
       </c>
@@ -1902,7 +1903,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>100</v>
       </c>
@@ -1916,7 +1917,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="6">
         <v>401</v>
       </c>
@@ -1924,7 +1925,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>101</v>
       </c>
@@ -1938,7 +1939,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>400</v>
       </c>
@@ -1949,7 +1950,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
         <v>400</v>
       </c>
@@ -1960,7 +1961,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
         <v>400</v>
       </c>
@@ -1971,7 +1972,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="6">
         <v>400</v>
       </c>
@@ -1982,7 +1983,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>111</v>
       </c>
@@ -1996,7 +1997,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" s="6">
         <v>400</v>
       </c>
@@ -2007,7 +2008,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" s="6">
         <v>404</v>
       </c>
@@ -2018,7 +2019,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>119</v>
       </c>
@@ -2032,7 +2033,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="6">
         <v>400</v>
       </c>
@@ -2046,7 +2047,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="6">
         <v>400</v>
       </c>
@@ -2060,7 +2061,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>117</v>
       </c>
@@ -2074,7 +2075,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="6">
         <v>400</v>
       </c>
@@ -2085,7 +2086,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="6">
         <v>400</v>
       </c>
@@ -2096,7 +2097,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="6">
         <v>400</v>
       </c>
@@ -2107,7 +2108,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="6">
         <v>400</v>
       </c>
@@ -2118,7 +2119,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" s="6">
         <v>400</v>
       </c>
@@ -2129,7 +2130,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="6">
         <v>401</v>
       </c>
@@ -2143,7 +2144,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="6">
         <v>401</v>
       </c>
@@ -2157,7 +2158,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" s="6">
         <v>401</v>
       </c>
@@ -2168,7 +2169,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B34" s="6">
         <v>401</v>
       </c>
@@ -2179,7 +2180,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>131</v>
       </c>
@@ -2193,7 +2194,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" s="6">
         <v>404</v>
       </c>
@@ -2204,7 +2205,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" s="6">
         <v>404</v>
       </c>
@@ -2215,7 +2216,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" s="6">
         <v>401</v>
       </c>
@@ -2226,7 +2227,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>134</v>
       </c>
@@ -2240,7 +2241,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" s="6">
         <v>404</v>
       </c>
@@ -2251,7 +2252,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" s="6">
         <v>404</v>
       </c>
@@ -2262,7 +2263,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>135</v>
       </c>
@@ -2276,7 +2277,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" s="6">
         <v>200</v>
       </c>
@@ -2287,7 +2288,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" s="6">
         <v>500</v>
       </c>
@@ -2298,7 +2299,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>139</v>
       </c>
@@ -2312,7 +2313,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B50" s="6">
         <v>404</v>
       </c>
@@ -2323,7 +2324,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B51" s="6">
         <v>404</v>
       </c>
@@ -2334,7 +2335,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>140</v>
       </c>
@@ -2348,7 +2349,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B54" s="6">
         <v>400</v>
       </c>
@@ -2359,7 +2360,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B55" s="6">
         <v>404</v>
       </c>
@@ -2370,7 +2371,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56" s="6">
         <v>404</v>
       </c>
@@ -2381,7 +2382,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B57" s="6">
         <v>401</v>
       </c>
@@ -2392,7 +2393,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>130</v>
       </c>
@@ -2406,7 +2407,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B60" s="6">
         <v>400</v>
       </c>
@@ -2417,7 +2418,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B61" s="6">
         <v>400</v>
       </c>
@@ -2428,7 +2429,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62" s="6">
         <v>400</v>
       </c>
@@ -2439,7 +2440,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B63" s="6">
         <v>401</v>
       </c>
@@ -2447,7 +2448,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>147</v>
       </c>
@@ -2464,7 +2465,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B66" s="6">
         <v>404</v>
       </c>
@@ -2475,7 +2476,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B67" s="6">
         <v>404</v>
       </c>
@@ -2486,7 +2487,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B68" s="6">
         <v>401</v>
       </c>
@@ -2497,7 +2498,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>152</v>
       </c>
@@ -2511,7 +2512,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B71" s="6">
         <v>404</v>
       </c>
@@ -2522,7 +2523,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B72" s="6">
         <v>404</v>
       </c>
@@ -2533,7 +2534,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>11</v>
       </c>
@@ -2547,7 +2548,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B75" s="6">
         <v>200</v>
       </c>
@@ -2558,7 +2559,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B76" s="6">
         <v>404</v>
       </c>
@@ -2569,7 +2570,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B77" s="6">
         <v>404</v>
       </c>
@@ -2580,7 +2581,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>155</v>
       </c>
@@ -2594,7 +2595,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B80" s="6">
         <v>400</v>
       </c>
@@ -2605,7 +2606,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B81" s="6">
         <v>400</v>
       </c>
@@ -2616,7 +2617,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B82" s="6">
         <v>400</v>
       </c>
@@ -2627,7 +2628,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B83" s="6">
         <v>401</v>
       </c>
@@ -2638,7 +2639,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B84" s="6">
         <v>401</v>
       </c>
@@ -2649,7 +2650,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B85" s="6">
         <v>404</v>
       </c>
@@ -2660,7 +2661,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>161</v>
       </c>
@@ -2674,7 +2675,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B88" s="6">
         <v>200</v>
       </c>
@@ -2685,7 +2686,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B89" s="6">
         <v>200</v>
       </c>
@@ -2696,7 +2697,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B90" s="6">
         <v>200</v>
       </c>
@@ -2707,7 +2708,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B91" s="6">
         <v>200</v>
       </c>
@@ -2718,7 +2719,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B92" s="6">
         <v>200</v>
       </c>
@@ -2729,7 +2730,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B93" s="6">
         <v>200</v>
       </c>
@@ -2740,7 +2741,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B94" s="6">
         <v>200</v>
       </c>
@@ -2751,7 +2752,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>60</v>
       </c>
@@ -2765,7 +2766,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="97" spans="2:4">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" s="6">
         <v>400</v>
       </c>
@@ -2776,7 +2777,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="98" spans="2:4">
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B98" s="6">
         <v>400</v>
       </c>
@@ -2787,7 +2788,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="99" spans="2:4">
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B99" s="6">
         <v>400</v>
       </c>

</xml_diff>

<commit_message>
24/07/2020 Update the excel file
</commit_message>
<xml_diff>
--- a/Restful-api.xlsx
+++ b/Restful-api.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\PycharmProjects\Restful-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA4BCC2-D9FF-49B9-AB40-9C21B54BA55A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9460B67B-4A03-43D2-8543-6892361DDE8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="2010" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{396F9068-CCEB-4AF1-BF68-127B62764BF9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="384">
   <si>
     <t>Function Name</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -946,490 +946,491 @@
     <t>EXIST_ALREADY</t>
   </si>
   <si>
+    <t>Null params</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_get_snap_status_code_200_by_null_params</t>
+  </si>
+  <si>
+    <t>test_get_snap_status_code_500_by_invalid_order_param</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_get_single_snap_status_code_400_by_missing_snap_id</t>
+  </si>
+  <si>
+    <t>test_get_single_snap_status_code_404_by_not_exist_snap_id</t>
+  </si>
+  <si>
+    <t>test_create_snap_status_code_201</t>
+  </si>
+  <si>
+    <t>test_create_snap_status_code_400_by_missing_title</t>
+  </si>
+  <si>
+    <t>test_create_snap_status_code_400_by_missing_description</t>
+  </si>
+  <si>
+    <t>test_create_snap_status_code_400_by_missing_image_name</t>
+  </si>
+  <si>
+    <t>test_create_snap_status_code_400_by_missing_image_body</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_create_snap_status_code_400_by_missing_ref_id</t>
+  </si>
+  <si>
+    <t>test_create_snap_status_code_400_by_image_size_9MB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_create_snap_status_code_400_by_image_size_11MB</t>
+  </si>
+  <si>
+    <t>test_create_snap_status_code_400_by_image_size_over_limit</t>
+  </si>
+  <si>
+    <t>test_create_snap_status_code_401_by_not_login</t>
+  </si>
+  <si>
+    <t>test_remove_snap_status_code_204</t>
+  </si>
+  <si>
+    <t>test_remove_snap_status_code_404_by_missing_snap_id</t>
+  </si>
+  <si>
+    <t>test_remove_snap_status_code_404_by_unexisting_snap_id</t>
+  </si>
+  <si>
+    <t>test_remove_snap_status_code_401_by_not_login</t>
+  </si>
+  <si>
+    <t>test_get_product_of_a_snap_status_code_200</t>
+  </si>
+  <si>
+    <t>test_get_product_of_a_snap_status_code_404_by_invalid_snap_id</t>
+  </si>
+  <si>
+    <t>test_search_snap_status_code_200</t>
+  </si>
+  <si>
+    <t>test_search_snap_status_code_200_by_empty_query</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_search_snap_status_code_500_by_incorrect_order_parameter</t>
+  </si>
+  <si>
+    <t>test_get_comments_of_a_snap_status_code_200</t>
+  </si>
+  <si>
+    <t>test_get_comments_of_a_snap_status_code_404_by_invalid_snap_id</t>
+  </si>
+  <si>
+    <t>test_post_comment_status_code_201</t>
+  </si>
+  <si>
+    <t>test_get_comments_of_a_snap_status_code_404_by_invalid_snap_id</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_post_comment_status_code_400_by_missing_comment</t>
+  </si>
+  <si>
+    <t>test_post_comment_status_code_404_by_invalid_snap_id</t>
+  </si>
+  <si>
+    <t>test_post_comment_status_code_401_by_not_login</t>
+  </si>
+  <si>
+    <t>test_get_snap_info_after_login_status_code_200</t>
+  </si>
+  <si>
+    <t>test_get_snap_info_after_login_status_code_400_by_missing_snap_id_for_home</t>
+  </si>
+  <si>
+    <t>test_get_snap_info_after_login_status_code_400_by_missing_snap_id_for_search</t>
+  </si>
+  <si>
+    <t>test_get_snap_info_after_login_status_code_400_by_missing_snap_id_for_product</t>
+  </si>
+  <si>
+    <t>test_get_snap_info_after_login_status_code_401_by_not_login_in</t>
+  </si>
+  <si>
+    <t>test_remove_a_snap_from_a_snap_status_code_204</t>
+  </si>
+  <si>
+    <t>test_remove_a_snap_from_a_snap_status_code_404_by_unexisting_snap_product_id</t>
+  </si>
+  <si>
+    <t>test_remove_a_snap_from_a_snap_status_code_404_by_missing_snap_product_id</t>
+  </si>
+  <si>
+    <t>test_remove_a_snap_from_a_snap_status_code_401_by_not_login</t>
+  </si>
+  <si>
+    <t>test_get_snaps_by_snap_product_id_status_code_200</t>
+  </si>
+  <si>
+    <t>test_get_snaps_by_snap_product_id_status_code_404_by_unexsiting_snap_product_id</t>
+  </si>
+  <si>
+    <t>test_get_snaps_by_snap_product_id_status_code_404_by_missing_snap_product_id</t>
+  </si>
+  <si>
+    <t>test_get_user_status_code_200</t>
+  </si>
+  <si>
+    <t>test_get_user_status_code_404_by_missing_user_id</t>
+  </si>
+  <si>
+    <t>test_change_password_status_code_200</t>
+  </si>
+  <si>
+    <t>test_change_password_status_code_400_by_missing_current_password</t>
+  </si>
+  <si>
+    <t>test_change_password_status_code_400_by_missing_new_password</t>
+  </si>
+  <si>
+    <t>test_change_password_status_code_401_by_unauthorized_user_id</t>
+  </si>
+  <si>
+    <t>test_change_password_status_code_400_by_invalid_new_password</t>
+  </si>
+  <si>
+    <t>test_change_password_status_code_401_by_not_login</t>
+  </si>
+  <si>
+    <t>test_change_password_status_code_404_by_invalid_current_password</t>
+  </si>
+  <si>
+    <t>test_update_user_profile_status_code_200</t>
+  </si>
+  <si>
+    <t>test_update_user_profile_status_code_400_by_invalid_username</t>
+  </si>
+  <si>
+    <t>test_update_user_profile_status_code_400_by_invalid_username</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_update_user_profile_status_code_400_by_invalid_bio</t>
+  </si>
+  <si>
+    <t>test_update_user_profile_status_code_401_by_not_login</t>
+  </si>
+  <si>
+    <t>test_update_user_profile_status_code_401_by_invalid_user_id</t>
+  </si>
+  <si>
+    <t>test_update_user_profile_picture_status_code_200_by_10kB</t>
+  </si>
+  <si>
+    <t>test_update_user_profile_picture_status_code_400_by_missing_image_name</t>
+  </si>
+  <si>
+    <t>4.5MB image</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_update_user_profile_picture_status_code_200_by_4_5MB_image</t>
+  </si>
+  <si>
+    <t>IMAGE_SIZE_OVER_LIMIT</t>
+  </si>
+  <si>
+    <t>IMAGE_SIZE_OVER_LIMIT</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_update_user_profile_picture_status_code_400_by_missing_image_body</t>
+  </si>
+  <si>
+    <t>test_update_user_profile_picture_status_code_401_by_unauthorized_user_id</t>
+  </si>
+  <si>
+    <t>test_update_user_profile_picture_status_code_401_by_not_login</t>
+  </si>
+  <si>
+    <t>test_update_user_profile_picture_status_code_404_by_invalid_image_body</t>
+  </si>
+  <si>
+    <t>test_remove_user_profile_picture_status_code_204</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_remove_user_profile_picture_status_code_401_by_invalid_user_id</t>
+  </si>
+  <si>
+    <t>test_remove_user_profile_picture_status_code_401_by_unauthorized_user_id</t>
+  </si>
+  <si>
+    <t>test_remove_user_profile_picture_status_code_401_by_not_login</t>
+  </si>
+  <si>
+    <t>test_follow_a_user_status_code_201</t>
+  </si>
+  <si>
+    <t>test_follow_a_user_status_code_401_by_not_login</t>
+  </si>
+  <si>
+    <t>test_follow_a_user_status_code_401_by_unauthorized_user_id</t>
+  </si>
+  <si>
+    <t>test_unfollow_a_user_status_code_204</t>
+  </si>
+  <si>
+    <t>test_unfollow_a_user_status_code_204_by_invalid_user_id</t>
+  </si>
+  <si>
+    <t>test_unfollow_a_user_status_code_400_by_unauthorized_user_id</t>
+  </si>
+  <si>
+    <t>test_unfollow_a_user_status_code_401_by_not_login</t>
+  </si>
+  <si>
+    <t>test_get_follower_status_code_200</t>
+  </si>
+  <si>
+    <t>test_get_follower_status_code_200_by_not_login</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_get_follower_status_code_200_by_unauthorized_user_id</t>
+  </si>
+  <si>
+    <t>test_get_follower_status_code_404_by_invalid_user_id</t>
+  </si>
+  <si>
+    <t>test_get_following_status_code_200</t>
+  </si>
+  <si>
+    <t>test_get_following_status_code_200_by_not_login</t>
+  </si>
+  <si>
+    <t>test_get_following_status_code_200_by_unauthorized_user_id</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_get_following_status_code_404_by_invalid_user_id</t>
+  </si>
+  <si>
+    <t>test_get_favourite_snaps_status_code_200</t>
+  </si>
+  <si>
+    <t>test_get_favourite_snaps_status_code_401_by_not_login</t>
+  </si>
+  <si>
+    <t>test_get_favourite_snaps_status_code_401_by_invalid_user_id</t>
+  </si>
+  <si>
+    <t>test_add_a_snap_to_favourite_status_code_201</t>
+  </si>
+  <si>
+    <t>test_add_a_snap_to_favourite_status_code_401_by_unauthorized_user_id</t>
+  </si>
+  <si>
+    <t>test_add_a_snap_to_favourite_status_code_401_by_not_login</t>
+  </si>
+  <si>
+    <t>test_remove_a_snap_from_favourite_status_code_204</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_remove_a_snap_to_favourite_status_code_204_by_invalid_snap_id</t>
+  </si>
+  <si>
+    <t>test_remove_a_snap_from_favourite_status_code_401_by_unauthorized_user_id</t>
+  </si>
+  <si>
+    <t>test_remove_a_snap_to_favourite_status_code_401_by_not_login</t>
+  </si>
+  <si>
+    <t>test_get_favourite_products_status_code_200</t>
+  </si>
+  <si>
+    <t>test_get_favourite_products_status_code_401_by_not_login</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_get_favourite_products_status_code_401_by_invalid_user_id</t>
+  </si>
+  <si>
+    <t>test_add_a_snap_product_to_favourite_status_code_201</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_add_a_product_to_favourite_status_code_401_by_unauthorized_user_id</t>
+  </si>
+  <si>
+    <t>test_add_a_product_to_favourite_status_code_401_by_not_login</t>
+  </si>
+  <si>
+    <t>test_add_a_product_to_favourite_status_code_401_by_invalid_snap_id</t>
+  </si>
+  <si>
+    <t>test_remove_a_product_from_favourite_status_code_204</t>
+  </si>
+  <si>
+    <t>test_remove_a_product_to_favourite_status_code_204_by_invalid_snap_id</t>
+  </si>
+  <si>
+    <t>test_remove_a_product_from_favourite_status_code_401_by_unauthorized_user_id</t>
+  </si>
+  <si>
+    <t>test_remove_a_product_to_favourite_status_code_401_by_not_login</t>
+  </si>
+  <si>
+    <t>test_get_snaps_of_a_user_status_code_200</t>
+  </si>
+  <si>
+    <t>test_get_snaps_of_a_user_status_code_200_by_unauthorized_user_id</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_get_snaps_of_a_user_status_code_200_by_not_login</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_get_snaps_of_a_user_status_code_404_by_invalid_user_id</t>
+  </si>
+  <si>
+    <t>test_get_snaps_of_a_user_status_code_500_by_invalid_order_param</t>
+  </si>
+  <si>
+    <t>test_forget_password_status_code_200</t>
+  </si>
+  <si>
+    <t>test_forget_password_status_code_400_by_missing_email</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_forget_password_status_code_400_by_invalid_email</t>
+  </si>
+  <si>
+    <t>test_report_a_user_status_code_201</t>
+  </si>
+  <si>
+    <t>test_report_a_user_status_code_201_by_not_login</t>
+  </si>
+  <si>
+    <t>test_report_a_user_status_code_201_by_self_user_id</t>
+  </si>
+  <si>
+    <t>test_report_a_user_status_code_201_by_missing_report_type</t>
+  </si>
+  <si>
+    <t>test_report_a_user_status_code_400_by_invalid_report_type</t>
+  </si>
+  <si>
+    <t>test_report_a_user_status_code_400_by_missing_user_id</t>
+  </si>
+  <si>
+    <t>test_report_a_user_status_code_404_by_invalid_user_id</t>
+  </si>
+  <si>
+    <t>test_check_username_valid_or_not_status_code_200_by_self_username</t>
+  </si>
+  <si>
+    <t>test_check_username_valid_or_not_status_code_200_by_unexisting_username</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_check_username_valid_or_not_status_code_400_by_invalid_username</t>
+  </si>
+  <si>
+    <t>test_check_username_valid_or_not_status_code_401_by_not_login</t>
+  </si>
+  <si>
+    <t>test_get_following_user_snaps_status_code_200</t>
+  </si>
+  <si>
+    <t>test_get_following_user_snaps_status_code_401_by_not_login</t>
+  </si>
+  <si>
+    <t>test_get_privacy_policy_status_code_200</t>
+  </si>
+  <si>
+    <t>test_get_terms_and_condition_status_code_200</t>
+  </si>
+  <si>
+    <t>test_get_getstart_background_image_status_code_200</t>
+  </si>
+  <si>
+    <t>test_social_media_list_status_code_200</t>
+  </si>
+  <si>
+    <t>test_get_snap_status_code_200</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET_FAIL</t>
+  </si>
+  <si>
+    <t>MISSING_TITLE</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>MISSING_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>MISSING_IMAGE_NAME</t>
+  </si>
+  <si>
+    <t>MISSING_IMAGE_BODY</t>
+  </si>
+  <si>
+    <t>MISSING_REF_ID</t>
+  </si>
+  <si>
+    <t>NOT_FOUND</t>
+  </si>
+  <si>
+    <t>NOT_FOUND</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>MISSING_SNAP_ID</t>
+  </si>
+  <si>
+    <t>MISSING_CURR_PASSWORD</t>
+  </si>
+  <si>
+    <t>MISSING_NEW_PASSWORD</t>
+  </si>
+  <si>
+    <t>INVALID_NEW_PASSWORD</t>
+  </si>
+  <si>
+    <t>UNAUTHORIZED</t>
+  </si>
+  <si>
+    <t>INVALID_USERNAME</t>
+  </si>
+  <si>
+    <t>INVALID_BIO</t>
+  </si>
+  <si>
+    <t>NOT_LOGIN</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>MISSING_IMAGE_BODY</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_follow_a_user_status_code_404_by_invalid_user_id</t>
+  </si>
+  <si>
+    <t>test_add_a_snap_to_favourite_status_code_404_by_invalid_snap_id</t>
+  </si>
+  <si>
     <t>test_get_single_snap_status_code_200</t>
-  </si>
-  <si>
-    <t>Null params</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_get_snap_status_code_200_by_null_params</t>
-  </si>
-  <si>
-    <t>test_get_snap_status_code_500_by_invalid_order_param</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_get_single_snap_status_code_400_by_missing_snap_id</t>
-  </si>
-  <si>
-    <t>test_get_single_snap_status_code_404_by_not_exist_snap_id</t>
-  </si>
-  <si>
-    <t>test_create_snap_status_code_201</t>
-  </si>
-  <si>
-    <t>test_create_snap_status_code_400_by_missing_title</t>
-  </si>
-  <si>
-    <t>test_create_snap_status_code_400_by_missing_description</t>
-  </si>
-  <si>
-    <t>test_create_snap_status_code_400_by_missing_image_name</t>
-  </si>
-  <si>
-    <t>test_create_snap_status_code_400_by_missing_image_body</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_create_snap_status_code_400_by_missing_ref_id</t>
-  </si>
-  <si>
-    <t>test_create_snap_status_code_400_by_image_size_9MB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_create_snap_status_code_400_by_image_size_11MB</t>
-  </si>
-  <si>
-    <t>test_create_snap_status_code_400_by_image_size_over_limit</t>
-  </si>
-  <si>
-    <t>test_create_snap_status_code_401_by_not_login</t>
-  </si>
-  <si>
-    <t>test_remove_snap_status_code_204</t>
-  </si>
-  <si>
-    <t>test_remove_snap_status_code_404_by_missing_snap_id</t>
-  </si>
-  <si>
-    <t>test_remove_snap_status_code_404_by_unexisting_snap_id</t>
-  </si>
-  <si>
-    <t>test_remove_snap_status_code_401_by_not_login</t>
-  </si>
-  <si>
-    <t>test_get_product_of_a_snap_status_code_200</t>
-  </si>
-  <si>
-    <t>test_get_product_of_a_snap_status_code_404_by_invalid_snap_id</t>
-  </si>
-  <si>
-    <t>test_search_snap_status_code_200</t>
-  </si>
-  <si>
-    <t>test_search_snap_status_code_200_by_empty_query</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_search_snap_status_code_500_by_incorrect_order_parameter</t>
-  </si>
-  <si>
-    <t>test_get_comments_of_a_snap_status_code_200</t>
-  </si>
-  <si>
-    <t>test_get_comments_of_a_snap_status_code_404_by_invalid_snap_id</t>
-  </si>
-  <si>
-    <t>test_post_comment_status_code_201</t>
-  </si>
-  <si>
-    <t>test_get_comments_of_a_snap_status_code_404_by_invalid_snap_id</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_post_comment_status_code_400_by_missing_comment</t>
-  </si>
-  <si>
-    <t>test_post_comment_status_code_404_by_invalid_snap_id</t>
-  </si>
-  <si>
-    <t>test_post_comment_status_code_401_by_not_login</t>
-  </si>
-  <si>
-    <t>test_get_snap_info_after_login_status_code_200</t>
-  </si>
-  <si>
-    <t>test_get_snap_info_after_login_status_code_400_by_missing_snap_id_for_home</t>
-  </si>
-  <si>
-    <t>test_get_snap_info_after_login_status_code_400_by_missing_snap_id_for_search</t>
-  </si>
-  <si>
-    <t>test_get_snap_info_after_login_status_code_400_by_missing_snap_id_for_product</t>
-  </si>
-  <si>
-    <t>test_get_snap_info_after_login_status_code_401_by_not_login_in</t>
-  </si>
-  <si>
-    <t>test_remove_a_snap_from_a_snap_status_code_204</t>
-  </si>
-  <si>
-    <t>test_remove_a_snap_from_a_snap_status_code_404_by_unexisting_snap_product_id</t>
-  </si>
-  <si>
-    <t>test_remove_a_snap_from_a_snap_status_code_404_by_missing_snap_product_id</t>
-  </si>
-  <si>
-    <t>test_remove_a_snap_from_a_snap_status_code_401_by_not_login</t>
-  </si>
-  <si>
-    <t>test_get_snaps_by_snap_product_id_status_code_200</t>
-  </si>
-  <si>
-    <t>test_get_snaps_by_snap_product_id_status_code_404_by_unexsiting_snap_product_id</t>
-  </si>
-  <si>
-    <t>test_get_snaps_by_snap_product_id_status_code_404_by_missing_snap_product_id</t>
-  </si>
-  <si>
-    <t>test_get_user_status_code_200</t>
-  </si>
-  <si>
-    <t>test_get_user_status_code_404_by_missing_user_id</t>
-  </si>
-  <si>
-    <t>test_change_password_status_code_200</t>
-  </si>
-  <si>
-    <t>test_change_password_status_code_400_by_missing_current_password</t>
-  </si>
-  <si>
-    <t>test_change_password_status_code_400_by_missing_new_password</t>
-  </si>
-  <si>
-    <t>test_change_password_status_code_401_by_unauthorized_user_id</t>
-  </si>
-  <si>
-    <t>test_change_password_status_code_400_by_invalid_new_password</t>
-  </si>
-  <si>
-    <t>test_change_password_status_code_401_by_not_login</t>
-  </si>
-  <si>
-    <t>test_change_password_status_code_404_by_invalid_current_password</t>
-  </si>
-  <si>
-    <t>test_update_user_profile_status_code_200</t>
-  </si>
-  <si>
-    <t>test_update_user_profile_status_code_400_by_invalid_username</t>
-  </si>
-  <si>
-    <t>test_update_user_profile_status_code_400_by_invalid_username</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_update_user_profile_status_code_400_by_invalid_bio</t>
-  </si>
-  <si>
-    <t>test_update_user_profile_status_code_401_by_not_login</t>
-  </si>
-  <si>
-    <t>test_update_user_profile_status_code_401_by_invalid_user_id</t>
-  </si>
-  <si>
-    <t>test_update_user_profile_picture_status_code_200_by_10kB</t>
-  </si>
-  <si>
-    <t>test_update_user_profile_picture_status_code_400_by_missing_image_name</t>
-  </si>
-  <si>
-    <t>4.5MB image</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_update_user_profile_picture_status_code_200_by_4_5MB_image</t>
-  </si>
-  <si>
-    <t>IMAGE_SIZE_OVER_LIMIT</t>
-  </si>
-  <si>
-    <t>IMAGE_SIZE_OVER_LIMIT</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_update_user_profile_picture_status_code_400_by_missing_image_body</t>
-  </si>
-  <si>
-    <t>test_update_user_profile_picture_status_code_401_by_unauthorized_user_id</t>
-  </si>
-  <si>
-    <t>test_update_user_profile_picture_status_code_401_by_not_login</t>
-  </si>
-  <si>
-    <t>test_update_user_profile_picture_status_code_404_by_invalid_image_body</t>
-  </si>
-  <si>
-    <t>test_remove_user_profile_picture_status_code_204</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_remove_user_profile_picture_status_code_401_by_invalid_user_id</t>
-  </si>
-  <si>
-    <t>test_remove_user_profile_picture_status_code_401_by_unauthorized_user_id</t>
-  </si>
-  <si>
-    <t>test_remove_user_profile_picture_status_code_401_by_not_login</t>
-  </si>
-  <si>
-    <t>test_follow_a_user_status_code_201</t>
-  </si>
-  <si>
-    <t>test_follow_a_user_status_code_401_by_not_login</t>
-  </si>
-  <si>
-    <t>test_follow_a_user_status_code_401_by_unauthorized_user_id</t>
-  </si>
-  <si>
-    <t>test_unfollow_a_user_status_code_204</t>
-  </si>
-  <si>
-    <t>test_unfollow_a_user_status_code_204_by_invalid_user_id</t>
-  </si>
-  <si>
-    <t>test_unfollow_a_user_status_code_400_by_unauthorized_user_id</t>
-  </si>
-  <si>
-    <t>test_unfollow_a_user_status_code_401_by_not_login</t>
-  </si>
-  <si>
-    <t>test_get_follower_status_code_200</t>
-  </si>
-  <si>
-    <t>test_get_follower_status_code_200_by_not_login</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_get_follower_status_code_200_by_unauthorized_user_id</t>
-  </si>
-  <si>
-    <t>test_get_follower_status_code_404_by_invalid_user_id</t>
-  </si>
-  <si>
-    <t>test_get_following_status_code_200</t>
-  </si>
-  <si>
-    <t>test_get_following_status_code_200_by_not_login</t>
-  </si>
-  <si>
-    <t>test_get_following_status_code_200_by_unauthorized_user_id</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_get_following_status_code_404_by_invalid_user_id</t>
-  </si>
-  <si>
-    <t>test_get_favourite_snaps_status_code_200</t>
-  </si>
-  <si>
-    <t>test_get_favourite_snaps_status_code_401_by_not_login</t>
-  </si>
-  <si>
-    <t>test_get_favourite_snaps_status_code_401_by_invalid_user_id</t>
-  </si>
-  <si>
-    <t>test_add_a_snap_to_favourite_status_code_201</t>
-  </si>
-  <si>
-    <t>test_add_a_snap_to_favourite_status_code_401_by_unauthorized_user_id</t>
-  </si>
-  <si>
-    <t>test_add_a_snap_to_favourite_status_code_401_by_not_login</t>
-  </si>
-  <si>
-    <t>test_remove_a_snap_from_favourite_status_code_204</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_remove_a_snap_to_favourite_status_code_204_by_invalid_snap_id</t>
-  </si>
-  <si>
-    <t>test_remove_a_snap_from_favourite_status_code_401_by_unauthorized_user_id</t>
-  </si>
-  <si>
-    <t>test_remove_a_snap_to_favourite_status_code_401_by_not_login</t>
-  </si>
-  <si>
-    <t>test_get_favourite_products_status_code_200</t>
-  </si>
-  <si>
-    <t>test_get_favourite_products_status_code_401_by_not_login</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_get_favourite_products_status_code_401_by_invalid_user_id</t>
-  </si>
-  <si>
-    <t>test_add_a_snap_product_to_favourite_status_code_201</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_add_a_product_to_favourite_status_code_401_by_unauthorized_user_id</t>
-  </si>
-  <si>
-    <t>test_add_a_product_to_favourite_status_code_401_by_not_login</t>
-  </si>
-  <si>
-    <t>test_add_a_product_to_favourite_status_code_401_by_invalid_snap_id</t>
-  </si>
-  <si>
-    <t>test_remove_a_product_from_favourite_status_code_204</t>
-  </si>
-  <si>
-    <t>test_remove_a_product_to_favourite_status_code_204_by_invalid_snap_id</t>
-  </si>
-  <si>
-    <t>test_remove_a_product_from_favourite_status_code_401_by_unauthorized_user_id</t>
-  </si>
-  <si>
-    <t>test_remove_a_product_to_favourite_status_code_401_by_not_login</t>
-  </si>
-  <si>
-    <t>test_get_snaps_of_a_user_status_code_200</t>
-  </si>
-  <si>
-    <t>test_get_snaps_of_a_user_status_code_200_by_unauthorized_user_id</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_get_snaps_of_a_user_status_code_200_by_not_login</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_get_snaps_of_a_user_status_code_404_by_invalid_user_id</t>
-  </si>
-  <si>
-    <t>test_get_snaps_of_a_user_status_code_500_by_invalid_order_param</t>
-  </si>
-  <si>
-    <t>test_forget_password_status_code_200</t>
-  </si>
-  <si>
-    <t>test_forget_password_status_code_400_by_missing_email</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_forget_password_status_code_400_by_invalid_email</t>
-  </si>
-  <si>
-    <t>test_report_a_user_status_code_201</t>
-  </si>
-  <si>
-    <t>test_report_a_user_status_code_201_by_not_login</t>
-  </si>
-  <si>
-    <t>test_report_a_user_status_code_201_by_self_user_id</t>
-  </si>
-  <si>
-    <t>test_report_a_user_status_code_201_by_missing_report_type</t>
-  </si>
-  <si>
-    <t>test_report_a_user_status_code_400_by_invalid_report_type</t>
-  </si>
-  <si>
-    <t>test_report_a_user_status_code_400_by_missing_user_id</t>
-  </si>
-  <si>
-    <t>test_report_a_user_status_code_404_by_invalid_user_id</t>
-  </si>
-  <si>
-    <t>test_check_username_valid_or_not_status_code_200_by_self_username</t>
-  </si>
-  <si>
-    <t>test_check_username_valid_or_not_status_code_200_by_unexisting_username</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_check_username_valid_or_not_status_code_400_by_invalid_username</t>
-  </si>
-  <si>
-    <t>test_check_username_valid_or_not_status_code_401_by_not_login</t>
-  </si>
-  <si>
-    <t>test_get_following_user_snaps_status_code_200</t>
-  </si>
-  <si>
-    <t>test_get_following_user_snaps_status_code_401_by_not_login</t>
-  </si>
-  <si>
-    <t>test_get_privacy_policy_status_code_200</t>
-  </si>
-  <si>
-    <t>test_get_terms_and_condition_status_code_200</t>
-  </si>
-  <si>
-    <t>test_get_getstart_background_image_status_code_200</t>
-  </si>
-  <si>
-    <t>test_social_media_list_status_code_200</t>
-  </si>
-  <si>
-    <t>test_get_snap_status_code_200</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>GET_FAIL</t>
-  </si>
-  <si>
-    <t>MISSING_TITLE</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>MISSING_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>MISSING_IMAGE_NAME</t>
-  </si>
-  <si>
-    <t>MISSING_IMAGE_BODY</t>
-  </si>
-  <si>
-    <t>MISSING_REF_ID</t>
-  </si>
-  <si>
-    <t>NOT_FOUND</t>
-  </si>
-  <si>
-    <t>NOT_FOUND</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>MISSING_SNAP_ID</t>
-  </si>
-  <si>
-    <t>MISSING_CURR_PASSWORD</t>
-  </si>
-  <si>
-    <t>MISSING_NEW_PASSWORD</t>
-  </si>
-  <si>
-    <t>INVALID_NEW_PASSWORD</t>
-  </si>
-  <si>
-    <t>UNAUTHORIZED</t>
-  </si>
-  <si>
-    <t>INVALID_USERNAME</t>
-  </si>
-  <si>
-    <t>INVALID_BIO</t>
-  </si>
-  <si>
-    <t>NOT_LOGIN</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>MISSING_IMAGE_BODY</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_follow_a_user_status_code_404_by_invalid_user_id</t>
-  </si>
-  <si>
-    <t>test_add_a_snap_to_favourite_status_code_404_by_invalid_snap_id</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2536,8 +2537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0FB8395-3546-4B63-9E36-2AC157E5E294}">
   <dimension ref="A1:G191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E119" sqref="E119"/>
+    <sheetView tabSelected="1" topLeftCell="A102" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2786,7 +2787,7 @@
         <v>111</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C17" s="6">
         <v>200</v>
@@ -2800,13 +2801,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C18" s="6">
         <v>200</v>
       </c>
       <c r="D18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>108</v>
@@ -2814,7 +2815,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C19" s="6">
         <v>500</v>
@@ -2823,7 +2824,7 @@
         <v>193</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>108</v>
@@ -2834,7 +2835,7 @@
         <v>119</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>230</v>
+        <v>383</v>
       </c>
       <c r="C21" s="6">
         <v>200</v>
@@ -2848,7 +2849,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C22" s="6">
         <v>400</v>
@@ -2865,7 +2866,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C23" s="6">
         <v>400</v>
@@ -2885,7 +2886,7 @@
         <v>117</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C26" s="6">
         <v>201</v>
@@ -2899,7 +2900,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C27" s="6">
         <v>400</v>
@@ -2908,7 +2909,7 @@
         <v>112</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>103</v>
@@ -2916,7 +2917,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C28" s="6">
         <v>400</v>
@@ -2925,7 +2926,7 @@
         <v>113</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>103</v>
@@ -2933,7 +2934,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C29" s="6">
         <v>400</v>
@@ -2942,7 +2943,7 @@
         <v>114</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>103</v>
@@ -2950,7 +2951,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C30" s="6">
         <v>400</v>
@@ -2959,7 +2960,7 @@
         <v>115</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>103</v>
@@ -2967,7 +2968,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C31" s="6">
         <v>400</v>
@@ -2976,7 +2977,7 @@
         <v>116</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>103</v>
@@ -2984,7 +2985,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C32" s="6">
         <v>401</v>
@@ -3002,7 +3003,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C33" s="6">
         <v>401</v>
@@ -3020,7 +3021,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C34" s="6">
         <v>401</v>
@@ -3029,7 +3030,7 @@
         <v>123</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>103</v>
@@ -3037,7 +3038,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C35" s="6">
         <v>401</v>
@@ -3057,7 +3058,7 @@
         <v>131</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C37" s="6">
         <v>204</v>
@@ -3071,7 +3072,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C38" s="6">
         <v>404</v>
@@ -3080,7 +3081,7 @@
         <v>118</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>103</v>
@@ -3088,7 +3089,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C39" s="6">
         <v>404</v>
@@ -3097,7 +3098,7 @@
         <v>120</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>103</v>
@@ -3105,7 +3106,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C40" s="6">
         <v>401</v>
@@ -3125,7 +3126,7 @@
         <v>134</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C42" s="6">
         <v>200</v>
@@ -3139,7 +3140,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C43" s="6">
         <v>404</v>
@@ -3148,7 +3149,7 @@
         <v>118</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>103</v>
@@ -3156,7 +3157,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C44" s="6">
         <v>404</v>
@@ -3165,7 +3166,7 @@
         <v>120</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>103</v>
@@ -3176,7 +3177,7 @@
         <v>135</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C46" s="6">
         <v>200</v>
@@ -3190,7 +3191,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C47" s="6">
         <v>200</v>
@@ -3204,7 +3205,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C48" s="6">
         <v>500</v>
@@ -3213,7 +3214,7 @@
         <v>138</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>103</v>
@@ -3224,7 +3225,7 @@
         <v>139</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C50" s="6">
         <v>200</v>
@@ -3238,7 +3239,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C51" s="6">
         <v>404</v>
@@ -3247,7 +3248,7 @@
         <v>118</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>103</v>
@@ -3255,7 +3256,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C52" s="6">
         <v>404</v>
@@ -3264,7 +3265,7 @@
         <v>137</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>103</v>
@@ -3275,7 +3276,7 @@
         <v>140</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C54" s="6">
         <v>201</v>
@@ -3289,7 +3290,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C55" s="6">
         <v>400</v>
@@ -3303,7 +3304,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C56" s="6">
         <v>404</v>
@@ -3312,7 +3313,7 @@
         <v>118</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>103</v>
@@ -3320,7 +3321,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C57" s="6">
         <v>404</v>
@@ -3329,7 +3330,7 @@
         <v>120</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>103</v>
@@ -3337,7 +3338,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C58" s="6">
         <v>401</v>
@@ -3357,7 +3358,7 @@
         <v>130</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C60" s="6">
         <v>200</v>
@@ -3371,7 +3372,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C61" s="6">
         <v>400</v>
@@ -3380,7 +3381,7 @@
         <v>143</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F61" s="6" t="s">
         <v>103</v>
@@ -3388,7 +3389,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C62" s="6">
         <v>400</v>
@@ -3397,7 +3398,7 @@
         <v>144</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F62" s="6" t="s">
         <v>103</v>
@@ -3405,7 +3406,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C63" s="6">
         <v>400</v>
@@ -3414,7 +3415,7 @@
         <v>145</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F63" s="6" t="s">
         <v>103</v>
@@ -3422,7 +3423,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C64" s="6">
         <v>401</v>
@@ -3442,7 +3443,7 @@
         <v>146</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C66" s="6">
         <v>204</v>
@@ -3459,7 +3460,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B67" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C67" s="6">
         <v>404</v>
@@ -3468,7 +3469,7 @@
         <v>148</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F67" s="6" t="s">
         <v>103</v>
@@ -3476,7 +3477,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B68" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C68" s="6">
         <v>404</v>
@@ -3485,7 +3486,7 @@
         <v>150</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F68" s="6" t="s">
         <v>103</v>
@@ -3493,7 +3494,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C69" s="6">
         <v>401</v>
@@ -3513,7 +3514,7 @@
         <v>151</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C71" s="6">
         <v>200</v>
@@ -3527,7 +3528,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C72" s="6">
         <v>404</v>
@@ -3536,7 +3537,7 @@
         <v>150</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F72" s="6" t="s">
         <v>103</v>
@@ -3544,7 +3545,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B73" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C73" s="6">
         <v>404</v>
@@ -3553,7 +3554,7 @@
         <v>148</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F73" s="6" t="s">
         <v>103</v>
@@ -3564,7 +3565,7 @@
         <v>11</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C75" s="6">
         <v>200</v>
@@ -3578,7 +3579,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B76" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C76" s="6">
         <v>200</v>
@@ -3592,7 +3593,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B77" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C77" s="6">
         <v>404</v>
@@ -3601,7 +3602,7 @@
         <v>152</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F77" s="6" t="s">
         <v>103</v>
@@ -3609,7 +3610,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C78" s="6">
         <v>404</v>
@@ -3618,7 +3619,7 @@
         <v>153</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F78" s="6" t="s">
         <v>103</v>
@@ -3629,7 +3630,7 @@
         <v>154</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C80" s="6">
         <v>200</v>
@@ -3643,7 +3644,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C81" s="6">
         <v>400</v>
@@ -3652,7 +3653,7 @@
         <v>155</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F81" s="6" t="s">
         <v>103</v>
@@ -3660,7 +3661,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C82" s="6">
         <v>400</v>
@@ -3669,7 +3670,7 @@
         <v>156</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F82" s="6" t="s">
         <v>103</v>
@@ -3677,7 +3678,7 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C83" s="6">
         <v>400</v>
@@ -3686,7 +3687,7 @@
         <v>158</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F83" s="6" t="s">
         <v>103</v>
@@ -3694,7 +3695,7 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C84" s="6">
         <v>401</v>
@@ -3703,7 +3704,7 @@
         <v>166</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F84" s="6" t="s">
         <v>103</v>
@@ -3711,7 +3712,7 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C85" s="6">
         <v>401</v>
@@ -3728,7 +3729,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C86" s="6">
         <v>404</v>
@@ -3737,7 +3738,7 @@
         <v>159</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F86" s="6" t="s">
         <v>103</v>
@@ -3748,7 +3749,7 @@
         <v>160</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C88" s="6">
         <v>200</v>
@@ -3762,7 +3763,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C89" s="6">
         <v>400</v>
@@ -3771,7 +3772,7 @@
         <v>161</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F89" s="6" t="s">
         <v>103</v>
@@ -3779,7 +3780,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C90" s="6">
         <v>400</v>
@@ -3788,7 +3789,7 @@
         <v>162</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F90" s="6" t="s">
         <v>103</v>
@@ -3796,7 +3797,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C91" s="6">
         <v>400</v>
@@ -3805,7 +3806,7 @@
         <v>163</v>
       </c>
       <c r="E91" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F91" s="6" t="s">
         <v>103</v>
@@ -3813,7 +3814,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C92" s="6">
         <v>401</v>
@@ -3822,7 +3823,7 @@
         <v>164</v>
       </c>
       <c r="E92" s="8" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F92" s="6" t="s">
         <v>103</v>
@@ -3830,7 +3831,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B93" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C93" s="6">
         <v>401</v>
@@ -3839,7 +3840,7 @@
         <v>166</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F93" s="6" t="s">
         <v>103</v>
@@ -3847,7 +3848,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B94" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C94" s="6">
         <v>401</v>
@@ -3856,7 +3857,7 @@
         <v>153</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F94" s="6" t="s">
         <v>103</v>
@@ -3864,7 +3865,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C95" s="6">
         <v>401</v>
@@ -3873,7 +3874,7 @@
         <v>165</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F95" s="6" t="s">
         <v>103</v>
@@ -3884,7 +3885,7 @@
         <v>60</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C97" s="6">
         <v>200</v>
@@ -3898,24 +3899,24 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B98" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C98" s="6">
         <v>200</v>
       </c>
       <c r="D98" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F98" s="6" t="s">
         <v>108</v>
       </c>
       <c r="G98" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C99" s="6">
         <v>400</v>
@@ -3924,7 +3925,7 @@
         <v>173</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F99" s="6" t="s">
         <v>103</v>
@@ -3932,7 +3933,7 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B100" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C100" s="6">
         <v>400</v>
@@ -3941,7 +3942,7 @@
         <v>171</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F100" s="6" t="s">
         <v>103</v>
@@ -3949,7 +3950,7 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B101" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C101" s="6">
         <v>401</v>
@@ -3958,7 +3959,7 @@
         <v>166</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F101" s="6" t="s">
         <v>103</v>
@@ -3966,7 +3967,7 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B102" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C102" s="6">
         <v>401</v>
@@ -3983,7 +3984,7 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B103" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C103" s="6">
         <v>404</v>
@@ -3992,7 +3993,7 @@
         <v>172</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F103" s="6" t="s">
         <v>103</v>
@@ -4003,7 +4004,7 @@
         <v>175</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C106" s="6">
         <v>204</v>
@@ -4017,7 +4018,7 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B107" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C107" s="6">
         <v>401</v>
@@ -4026,7 +4027,7 @@
         <v>177</v>
       </c>
       <c r="E107" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F107" s="6" t="s">
         <v>103</v>
@@ -4034,7 +4035,7 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C108" s="6">
         <v>401</v>
@@ -4043,7 +4044,7 @@
         <v>166</v>
       </c>
       <c r="E108" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F108" s="6" t="s">
         <v>103</v>
@@ -4051,7 +4052,7 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B109" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C109" s="6">
         <v>401</v>
@@ -4071,7 +4072,7 @@
         <v>179</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C111" s="6">
         <v>201</v>
@@ -4085,7 +4086,7 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B112" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C112" s="6">
         <v>401</v>
@@ -4102,7 +4103,7 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B113" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C113" s="6">
         <v>401</v>
@@ -4111,7 +4112,7 @@
         <v>166</v>
       </c>
       <c r="E113" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F113" s="6" t="s">
         <v>103</v>
@@ -4119,7 +4120,7 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B114" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C114" s="6">
         <v>404</v>
@@ -4128,7 +4129,7 @@
         <v>165</v>
       </c>
       <c r="E114" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F114" s="6" t="s">
         <v>103</v>
@@ -4139,7 +4140,7 @@
         <v>182</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C116" s="6">
         <v>204</v>
@@ -4153,7 +4154,7 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C117" s="6">
         <v>204</v>
@@ -4168,7 +4169,7 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B118" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C118" s="6">
         <v>400</v>
@@ -4177,7 +4178,7 @@
         <v>166</v>
       </c>
       <c r="E118" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F118" s="6" t="s">
         <v>103</v>
@@ -4185,7 +4186,7 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B119" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C119" s="6">
         <v>401</v>
@@ -4205,7 +4206,7 @@
         <v>184</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C121" s="6">
         <v>200</v>
@@ -4219,7 +4220,7 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B122" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C122" s="6">
         <v>200</v>
@@ -4234,7 +4235,7 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B123" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C123" s="6">
         <v>200</v>
@@ -4249,7 +4250,7 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B124" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C124" s="6">
         <v>404</v>
@@ -4258,7 +4259,7 @@
         <v>165</v>
       </c>
       <c r="E124" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F124" s="6" t="s">
         <v>103</v>
@@ -4269,7 +4270,7 @@
         <v>186</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C126" s="6">
         <v>200</v>
@@ -4283,7 +4284,7 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B127" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C127" s="6">
         <v>200</v>
@@ -4297,7 +4298,7 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B128" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C128" s="6">
         <v>200</v>
@@ -4311,7 +4312,7 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B129" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C129" s="6">
         <v>404</v>
@@ -4320,7 +4321,7 @@
         <v>165</v>
       </c>
       <c r="E129" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F129" s="6" t="s">
         <v>103</v>
@@ -4331,7 +4332,7 @@
         <v>187</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C131" s="6">
         <v>200</v>
@@ -4345,7 +4346,7 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B132" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C132" s="6">
         <v>401</v>
@@ -4362,7 +4363,7 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B133" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C133" s="6">
         <v>401</v>
@@ -4371,7 +4372,7 @@
         <v>177</v>
       </c>
       <c r="E133" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F133" s="6" t="s">
         <v>103</v>
@@ -4382,7 +4383,7 @@
         <v>76</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C135" s="6">
         <v>201</v>
@@ -4396,7 +4397,7 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B136" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C136" s="6">
         <v>401</v>
@@ -4405,7 +4406,7 @@
         <v>166</v>
       </c>
       <c r="E136" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F136" s="6" t="s">
         <v>103</v>
@@ -4413,7 +4414,7 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B137" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C137" s="6">
         <v>401</v>
@@ -4430,7 +4431,7 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B138" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C138" s="6">
         <v>404</v>
@@ -4439,7 +4440,7 @@
         <v>165</v>
       </c>
       <c r="E138" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F138" s="6" t="s">
         <v>103</v>
@@ -4450,7 +4451,7 @@
         <v>189</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C140" s="6">
         <v>204</v>
@@ -4464,7 +4465,7 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B141" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C141" s="6">
         <v>204</v>
@@ -4478,7 +4479,7 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B142" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C142" s="6">
         <v>401</v>
@@ -4486,19 +4487,25 @@
       <c r="D142" t="s">
         <v>166</v>
       </c>
+      <c r="E142" s="8" t="s">
+        <v>376</v>
+      </c>
       <c r="F142" s="6" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B143" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C143" s="6">
         <v>401</v>
       </c>
       <c r="D143" t="s">
         <v>188</v>
+      </c>
+      <c r="E143" s="8" t="s">
+        <v>224</v>
       </c>
       <c r="F143" s="6" t="s">
         <v>103</v>
@@ -4509,7 +4516,7 @@
         <v>190</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C145" s="6">
         <v>200</v>
@@ -4523,7 +4530,7 @@
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B146" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C146" s="6">
         <v>401</v>
@@ -4531,19 +4538,25 @@
       <c r="D146" t="s">
         <v>185</v>
       </c>
+      <c r="E146" s="8" t="s">
+        <v>224</v>
+      </c>
       <c r="F146" s="6" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B147" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C147" s="6">
         <v>401</v>
       </c>
       <c r="D147" t="s">
         <v>177</v>
+      </c>
+      <c r="E147" s="8" t="s">
+        <v>376</v>
       </c>
       <c r="F147" s="6" t="s">
         <v>103</v>
@@ -4554,7 +4567,7 @@
         <v>82</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C149" s="6">
         <v>201</v>
@@ -4568,7 +4581,7 @@
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B150" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C150" s="6">
         <v>401</v>
@@ -4576,13 +4589,16 @@
       <c r="D150" t="s">
         <v>166</v>
       </c>
+      <c r="E150" s="8" t="s">
+        <v>376</v>
+      </c>
       <c r="F150" s="6" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B151" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C151" s="6">
         <v>401</v>
@@ -4590,19 +4606,25 @@
       <c r="D151" t="s">
         <v>188</v>
       </c>
+      <c r="E151" s="8" t="s">
+        <v>224</v>
+      </c>
       <c r="F151" s="6" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B152" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C152" s="6">
         <v>401</v>
       </c>
       <c r="D152" t="s">
         <v>165</v>
+      </c>
+      <c r="E152" s="8" t="s">
+        <v>376</v>
       </c>
       <c r="F152" s="6" t="s">
         <v>103</v>
@@ -4613,7 +4635,7 @@
         <v>191</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C154" s="6">
         <v>204</v>
@@ -4627,7 +4649,7 @@
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B155" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C155" s="6">
         <v>204</v>
@@ -4641,7 +4663,7 @@
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B156" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C156" s="6">
         <v>401</v>
@@ -4655,7 +4677,7 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B157" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C157" s="6">
         <v>401</v>
@@ -4672,7 +4694,7 @@
         <v>192</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C159" s="6">
         <v>200</v>
@@ -4686,7 +4708,7 @@
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B160" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C160" s="6">
         <v>200</v>
@@ -4700,7 +4722,7 @@
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B161" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C161" s="6">
         <v>200</v>
@@ -4714,7 +4736,7 @@
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B162" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C162" s="6">
         <v>404</v>
@@ -4728,7 +4750,7 @@
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B163" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C163" s="6">
         <v>500</v>
@@ -4745,7 +4767,7 @@
         <v>194</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C165" s="6">
         <v>200</v>
@@ -4759,7 +4781,7 @@
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B166" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C166" s="6">
         <v>400</v>
@@ -4773,7 +4795,7 @@
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B167" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C167" s="6">
         <v>400</v>
@@ -4790,7 +4812,7 @@
         <v>196</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C169" s="6">
         <v>201</v>
@@ -4804,7 +4826,7 @@
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B170" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C170" s="6">
         <v>201</v>
@@ -4818,7 +4840,7 @@
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B171" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C171" s="6">
         <v>201</v>
@@ -4832,7 +4854,7 @@
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B172" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C172" s="6">
         <v>201</v>
@@ -4846,7 +4868,7 @@
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B173" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C173" s="6">
         <v>400</v>
@@ -4860,7 +4882,7 @@
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B174" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C174" s="6">
         <v>400</v>
@@ -4874,7 +4896,7 @@
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B175" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C175" s="6">
         <v>404</v>
@@ -4891,7 +4913,7 @@
         <v>201</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C177" s="6">
         <v>200</v>
@@ -4905,7 +4927,7 @@
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B178" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C178" s="6">
         <v>200</v>
@@ -4919,7 +4941,7 @@
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B179" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C179" s="6">
         <v>400</v>
@@ -4933,7 +4955,7 @@
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B180" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C180" s="6">
         <v>401</v>
@@ -4950,7 +4972,7 @@
         <v>206</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C182" s="6">
         <v>200</v>
@@ -4964,7 +4986,7 @@
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B183" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C183" s="6">
         <v>401</v>
@@ -4981,7 +5003,7 @@
         <v>207</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C185" s="6">
         <v>200</v>
@@ -4998,7 +5020,7 @@
         <v>208</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C187" s="6">
         <v>200</v>
@@ -5015,7 +5037,7 @@
         <v>209</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C189" s="6">
         <v>200</v>
@@ -5032,7 +5054,7 @@
         <v>210</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C191" s="6">
         <v>200</v>

</xml_diff>

<commit_message>
Update the Restful-api.xlsx & README.md
</commit_message>
<xml_diff>
--- a/Restful-api.xlsx
+++ b/Restful-api.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\PycharmProjects\Restful-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E655F585-D26B-4FE6-9E40-7D4114DB7433}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30D6242-8026-46BB-8F82-E35C97128FB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{396F9068-CCEB-4AF1-BF68-127B62764BF9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{396F9068-CCEB-4AF1-BF68-127B62764BF9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Complex Test Case" sheetId="1" r:id="rId1"/>
+    <sheet name="Complex Test Case - Past" sheetId="1" r:id="rId1"/>
     <sheet name="Complex Test Case - Updated" sheetId="3" r:id="rId2"/>
     <sheet name="Unit Test Case" sheetId="2" r:id="rId3"/>
   </sheets>
@@ -1880,7 +1880,7 @@
   <dimension ref="A1:C136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:B20"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2496,6 +2496,7 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2504,7 +2505,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2624,8 +2625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0FB8395-3546-4B63-9E36-2AC157E5E294}">
   <dimension ref="A1:H202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F194" sqref="F194"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>

</xml_diff>